<commit_message>
New library updated has been done. Thread sleep statement changed with expected conditions.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/testdata.xlsx
+++ b/src/test/java/resources/testdata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -61,12 +61,16 @@
   </si>
   <si>
     <t>E-posta adresiniz veya şifreniz hatalı</t>
+  </si>
+  <si>
+    <t>PASSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -479,12 +483,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="5" width="45.0" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="6" width="25.5703125" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="6" width="12.0" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="6" width="28.42578125" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="32.42578125" collapsed="false"/>
+    <col min="6" max="10" customWidth="true" width="20.7109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -521,7 +525,9 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -535,7 +541,9 @@
       <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>

</xml_diff>